<commit_message>
Country of Birth added to patient profile
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-historical-data.xlsx
+++ b/output/StructureDefinition-historical-data.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="66">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-11T17:34:16+02:00</t>
+    <t>2023-07-13T10:52:26+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -165,21 +165,11 @@
     <t>Extension.extension</t>
   </si>
   <si>
-    <t>extensions
-user content</t>
-  </si>
-  <si>
     <t xml:space="preserve">Extension
 </t>
   </si>
   <si>
-    <t>Additional content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
+    <t>An Extension</t>
   </si>
   <si>
     <t xml:space="preserve">value:url}
@@ -219,10 +209,6 @@
   </si>
   <si>
     <t>Extension.value[x]</t>
-  </si>
-  <si>
-    <t>base64Binary
-booleancanonicalcodedatedateTimedecimalidinstantintegermarkdownoidpositiveIntstringtimeunsignedInturiurluuidAddressAgeAnnotationAttachmentCodeableConceptCodingContactPointCountDistanceDurationHumanNameIdentifierMoneyPeriodQuantityRangeRatioReferenceSampledDataSignatureTimingContactDetailContributorDataRequirementExpressionParameterDefinitionRelatedArtifactTriggerDefinitionUsageContextDosageMeta</t>
   </si>
   <si>
     <t>Value of extension</t>
@@ -546,13 +532,13 @@
   <cols>
     <col min="1" max="1" width="19.03515625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="19.03515625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.203125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="1.04296875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="6" max="6" width="2.203125" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="2.203125" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="255.0" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="9.734375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -795,14 +781,14 @@
       </c>
       <c r="C3" s="2"/>
       <c r="D3" t="s" s="2">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" t="s" s="2">
         <v>37</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" t="s" s="2">
         <v>36</v>
@@ -814,17 +800,15 @@
         <v>36</v>
       </c>
       <c r="K3" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="L3" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="M3" t="s" s="2">
         <v>50</v>
       </c>
-      <c r="L3" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="M3" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="N3" t="s" s="2">
-        <v>53</v>
-      </c>
+      <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" t="s" s="2">
         <v>36</v>
@@ -861,19 +845,19 @@
         <v>36</v>
       </c>
       <c r="AB3" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AC3" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AD3" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AE3" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AF3" t="s" s="2">
         <v>54</v>
-      </c>
-      <c r="AC3" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="AD3" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AE3" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AF3" t="s" s="2">
-        <v>57</v>
       </c>
       <c r="AG3" t="s" s="2">
         <v>37</v>
@@ -885,18 +869,18 @@
         <v>36</v>
       </c>
       <c r="AJ3" t="s" s="2">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AK3" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" t="s" s="2">
@@ -919,16 +903,16 @@
         <v>36</v>
       </c>
       <c r="K4" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="L4" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="M4" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="N4" t="s" s="2">
         <v>60</v>
-      </c>
-      <c r="L4" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="M4" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="N4" t="s" s="2">
-        <v>63</v>
       </c>
       <c r="O4" s="2"/>
       <c r="P4" t="s" s="2">
@@ -978,7 +962,7 @@
         <v>36</v>
       </c>
       <c r="AF4" t="s" s="2">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AG4" t="s" s="2">
         <v>42</v>
@@ -993,15 +977,15 @@
         <v>36</v>
       </c>
       <c r="AK4" t="s" s="2">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s" s="2">
@@ -1024,13 +1008,13 @@
         <v>36</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -1081,7 +1065,7 @@
         <v>36</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="AG5" t="s" s="2">
         <v>37</v>
@@ -1093,10 +1077,10 @@
         <v>36</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="AK5" t="s" s="2">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>